<commit_message>
All teh datasets from WPF with their associated json data
</commit_message>
<xml_diff>
--- a/DataSets/Holidays.xlsx
+++ b/DataSets/Holidays.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Adaptable Samples\AdaptableSamples\Holidays\Spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Source\Repos\adaptableblotter-demo\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4095,10 +4095,10 @@
   <dimension ref="A1:IV1014"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C989" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1006" sqref="I1006"/>
+      <selection pane="bottomRight" activeCell="E1005" sqref="E1005"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>